<commit_message>
last commit for 051822
</commit_message>
<xml_diff>
--- a/Data/results/question_3.xlsx
+++ b/Data/results/question_3.xlsx
@@ -573,7 +573,7 @@
         <v>14.638</v>
       </c>
       <c r="B2">
-        <v>22.1522499169223</v>
+        <v>22.15224991692185</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -597,7 +597,7 @@
         <v>10.585</v>
       </c>
       <c r="B5">
-        <v>24.62636796537572</v>
+        <v>24.62636796537527</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -605,7 +605,7 @@
         <v>19.99571428571429</v>
       </c>
       <c r="B6">
-        <v>18.31977188823794</v>
+        <v>18.31977188823703</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -621,7 +621,7 @@
         <v>22.2475</v>
       </c>
       <c r="B8">
-        <v>19.28718229407968</v>
+        <v>19.28718229407923</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -637,7 +637,7 @@
         <v>6.285</v>
       </c>
       <c r="B10">
-        <v>14.93120691803188</v>
+        <v>14.93120691803142</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -645,7 +645,7 @@
         <v>20.23333333333333</v>
       </c>
       <c r="B11">
-        <v>19.5550548622391</v>
+        <v>19.55505486223956</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -677,7 +677,7 @@
         <v>23.25409090909091</v>
       </c>
       <c r="B15">
-        <v>14.1501079892837</v>
+        <v>14.15010798928279</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -693,7 +693,7 @@
         <v>15.8</v>
       </c>
       <c r="B17">
-        <v>22.23853536337674</v>
+        <v>22.23853536337629</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -709,7 +709,7 @@
         <v>17.25833333333333</v>
       </c>
       <c r="B19">
-        <v>24.41798080766557</v>
+        <v>24.41798080766603</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -717,7 +717,7 @@
         <v>17.8085</v>
       </c>
       <c r="B20">
-        <v>22.9431547212057</v>
+        <v>22.94315472120525</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -725,7 +725,7 @@
         <v>15.19</v>
       </c>
       <c r="B21">
-        <v>10.80159348165353</v>
+        <v>10.80159348165398</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -741,7 +741,7 @@
         <v>18.01444444444444</v>
       </c>
       <c r="B23">
-        <v>20.1299677719071</v>
+        <v>20.12996777190756</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -749,7 +749,7 @@
         <v>12.35</v>
       </c>
       <c r="B24">
-        <v>21.6701039042423</v>
+        <v>21.67010390424139</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -757,7 +757,7 @@
         <v>14.88857142857143</v>
       </c>
       <c r="B25">
-        <v>16.71100678809717</v>
+        <v>16.71100678809626</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -765,7 +765,7 @@
         <v>17.53</v>
       </c>
       <c r="B26">
-        <v>22.32765813163996</v>
+        <v>22.32765813164042</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -773,7 +773,7 @@
         <v>21.43</v>
       </c>
       <c r="B27">
-        <v>15.61595102508409</v>
+        <v>15.61595102508363</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -781,7 +781,7 @@
         <v>17.66428571428571</v>
       </c>
       <c r="B28">
-        <v>24.12430802630024</v>
+        <v>24.12430802629979</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -789,7 +789,7 @@
         <v>22.35285714285714</v>
       </c>
       <c r="B29">
-        <v>21.31762274053744</v>
+        <v>21.31762274053654</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -805,7 +805,7 @@
         <v>18.97545454545454</v>
       </c>
       <c r="B31">
-        <v>15.33893342811189</v>
+        <v>15.33893342811052</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -813,7 +813,7 @@
         <v>19.42</v>
       </c>
       <c r="B32">
-        <v>18.29875251871408</v>
+        <v>18.29875251871454</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -821,7 +821,7 @@
         <v>26</v>
       </c>
       <c r="B33">
-        <v>17.62610086942277</v>
+        <v>17.62610086942232</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -829,7 +829,7 @@
         <v>29.46</v>
       </c>
       <c r="B34">
-        <v>21.85289334376603</v>
+        <v>21.85289334376557</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -837,7 +837,7 @@
         <v>25.76</v>
       </c>
       <c r="B35">
-        <v>20.56361354442015</v>
+        <v>20.56361354441924</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -845,7 +845,7 @@
         <v>20.095</v>
       </c>
       <c r="B36">
-        <v>13.23981160907442</v>
+        <v>13.23981160907397</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -853,7 +853,7 @@
         <v>11.115</v>
       </c>
       <c r="B37">
-        <v>21.90151061219376</v>
+        <v>21.90151061219422</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -861,7 +861,7 @@
         <v>18.29</v>
       </c>
       <c r="B38">
-        <v>22.81836141368876</v>
+        <v>22.81836141368831</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -869,7 +869,7 @@
         <v>21.55</v>
       </c>
       <c r="B39">
-        <v>21.55900454306629</v>
+        <v>21.5590045430672</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -893,7 +893,7 @@
         <v>19.995</v>
       </c>
       <c r="B42">
-        <v>21.24899885130526</v>
+        <v>21.2489988513048</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -909,7 +909,7 @@
         <v>24.17</v>
       </c>
       <c r="B44">
-        <v>28.24007690650706</v>
+        <v>28.24007690650615</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -917,7 +917,7 @@
         <v>19.08</v>
       </c>
       <c r="B45">
-        <v>21.48676651013284</v>
+        <v>21.48676651013329</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -925,7 +925,7 @@
         <v>15.05</v>
       </c>
       <c r="B46">
-        <v>10.59297773533808</v>
+        <v>10.59297773533854</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -933,7 +933,7 @@
         <v>21.804</v>
       </c>
       <c r="B47">
-        <v>22.90429674374172</v>
+        <v>22.90429674374082</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -941,7 +941,7 @@
         <v>20.43916666666667</v>
       </c>
       <c r="B48">
-        <v>15.98519858054715</v>
+        <v>15.9851985805476</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -957,7 +957,7 @@
         <v>22.745</v>
       </c>
       <c r="B50">
-        <v>19.26704491116561</v>
+        <v>19.2670449111688</v>
       </c>
     </row>
   </sheetData>

</xml_diff>